<commit_message>
Test new parameters for corrected code
</commit_message>
<xml_diff>
--- a/data/roads_parameters.xlsx
+++ b/data/roads_parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>GDB-Code</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>3 m Strasse</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Route 3m. Route secondaire étroite et, la plus part du temps, praticable pour tous véhicules. Certaines routes non praticables peuvent être plus larges.&amp;#10;Largeur: &gt; 2.81 m – 4.20 m.&amp;#10;Longueur minimale: 50 m&amp;#10;(+) Tronçons non praticable avec une largeur variable &gt; 2.80 m&amp;#10;(-) Route agricole autour des fermes</t>
@@ -120,7 +123,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,12 +134,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -188,11 +185,11 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -694,10 +691,10 @@
         <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="6">
         <v>3.4</v>
@@ -708,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>6</v>
@@ -721,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -734,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -747,7 +744,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>6</v>
@@ -762,7 +759,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>6</v>
@@ -777,7 +774,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>6</v>
@@ -790,7 +787,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>6</v>
@@ -805,7 +802,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>6</v>
@@ -818,13 +815,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="3">
         <v>10</v>
@@ -835,7 +832,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>6</v>
@@ -850,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>6</v>
@@ -863,7 +860,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Filter roads by type in assessment
</commit_message>
<xml_diff>
--- a/data/roads_parameters.xlsx
+++ b/data/roads_parameters.xlsx
@@ -70,7 +70,7 @@
     <t>Route 4m. Routes secondaires bien aménagées (signalisée en blanc) ainsi que les routes de quartier sur lesquelles deux voitures peuvent se croiser pratiquement partout.&amp;#10;Largeur: 4.21 m – 6.20 m.&amp;#10;Longueur minimale: 50 m</t>
   </si>
   <si>
-    <t>3 m Strasse</t>
+    <t>3m Strasse</t>
   </si>
   <si>
     <t>yes</t>
@@ -88,10 +88,10 @@
     <t>Fahere</t>
   </si>
   <si>
-    <t>2 m Weg</t>
-  </si>
-  <si>
-    <t>1 m Weg</t>
+    <t>2m Weg</t>
+  </si>
+  <si>
+    <t>1m Weg</t>
   </si>
   <si>
     <t>1 m Wegfagment</t>
@@ -619,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -634,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -649,7 +649,7 @@
         <v>10.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="44.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -666,7 +666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="44.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -683,7 +683,7 @@
         <v>5.21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="73.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="69.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -700,7 +700,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -713,7 +713,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -726,7 +726,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -739,7 +739,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -747,14 +747,14 @@
         <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6">
         <v>1.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -762,14 +762,14 @@
         <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -782,7 +782,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="44.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -842,7 +842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -868,21 +868,21 @@
       <c r="D24" s="5"/>
       <c r="E24" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="7"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="7"/>
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="E26" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="7"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>

</xml_diff>